<commit_message>
decision tree assignment ver 2
decision tree assignment
</commit_message>
<xml_diff>
--- a/DecisionTree_model_results.xlsx
+++ b/DecisionTree_model_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a614c51e60243dc/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{6E747670-3FF7-4B20-8C28-C8AB9C801A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2DD8078-6034-4077-8D54-E41DF1A27100}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{6E747670-3FF7-4B20-8C28-C8AB9C801A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34D37A0E-4610-4F00-87FD-358759696B82}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="741" xr2:uid="{411D9533-0127-4F3E-8B06-4A8E0E5231B2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="806" xr2:uid="{411D9533-0127-4F3E-8B06-4A8E0E5231B2}"/>
   </bookViews>
   <sheets>
     <sheet name="overall_results_list" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>criterion</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>poisson_</t>
+  </si>
+  <si>
+    <t>got best result</t>
+  </si>
+  <si>
+    <t>Result Desc</t>
   </si>
 </sst>
 </file>
@@ -443,13 +449,18 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAD4FCD5-7124-471F-AF39-A01A74BBDE14}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{EAD4FCD5-7124-471F-AF39-A01A74BBDE14}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EAD4FCD5-7124-471F-AF39-A01A74BBDE14}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{EAD4FCD5-7124-471F-AF39-A01A74BBDE14}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{EF6FE3E3-25C1-46C0-8500-79057F0031B2}" name="criterion"/>
     <tableColumn id="2" xr3:uid="{366CC974-59C3-4F2A-BF14-8ECBDB0C243C}" name="splitter"/>
     <tableColumn id="3" xr3:uid="{FBDBF098-6B37-4D0D-A649-93062066C887}" name="r_score"/>
+    <tableColumn id="4" xr3:uid="{EF37E11C-8201-4940-ADE3-AED170356B55}" name="Result Desc"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -772,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E10E2A-F32D-4F54-BB2B-CD9267CF50C9}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -783,9 +794,10 @@
     <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.90625" customWidth="1"/>
     <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,8 +807,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -807,7 +822,7 @@
         <v>0.90305439049749903</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -818,7 +833,7 @@
         <v>0.90305439049749903</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -829,7 +844,7 @@
         <v>0.85769521663967596</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -840,7 +855,7 @@
         <v>0.90957997597593898</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -850,8 +865,11 @@
       <c r="C6" s="2">
         <v>0.95195752281488299</v>
       </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -862,7 +880,7 @@
         <v>0.86676511625661601</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -873,7 +891,7 @@
         <v>0.91621946672775101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>

</xml_diff>